<commit_message>
kompletly rewrote the GED base SVC's
</commit_message>
<xml_diff>
--- a/configs/results/initial_test_run_MUTAG_results.xlsx
+++ b/configs/results/initial_test_run_MUTAG_results.xlsx
@@ -55,11 +55,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -425,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V1"/>
+  <dimension ref="A1:V21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -545,6 +546,1846 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" s="2" t="n">
+        <v>4.060185185185185e-07</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>SVC_WeisfeilerLehman_5_precomputed</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="D2" s="2" t="n">
+        <v>2.130974537037037e-05</v>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>{'C': 0.75, 'class_weight': 'balanced', 'kernel_type': 'precomputed', 'n_iter': 1}</t>
+        </is>
+      </c>
+      <c r="F2" t="n">
+        <v>0.7333333333333334</v>
+      </c>
+      <c r="G2" s="2" t="n">
+        <v>4.082523148148148e-07</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0.09578947368421054</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0.08972897632394194</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0.06144019379313492</v>
+      </c>
+      <c r="K2" t="n">
+        <v>0.6842105263157895</v>
+      </c>
+      <c r="L2" t="n">
+        <v>0.6949760765550239</v>
+      </c>
+      <c r="M2" t="n">
+        <v>0.7243589743589745</v>
+      </c>
+      <c r="N2" t="n">
+        <v>0.78</v>
+      </c>
+      <c r="O2" t="n">
+        <v>0.7847050528789659</v>
+      </c>
+      <c r="P2" t="n">
+        <v>0.7857991681521094</v>
+      </c>
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">              precision    recall  f1-score   support
+          -1       0.50      0.83      0.62        12
+           1       0.89      0.62      0.73        26
+    accuracy                           0.68        38
+   macro avg       0.69      0.72      0.68        38
+weighted avg       0.77      0.68      0.69        38
+</t>
+        </is>
+      </c>
+      <c r="R2" t="inlineStr">
+        <is>
+          <t>0.7341394025604553 ∓ 0.031950041839222024</t>
+        </is>
+      </c>
+      <c r="S2" t="inlineStr">
+        <is>
+          <t>0.7377316924069289 ∓ 0.03169216459652803</t>
+        </is>
+      </c>
+      <c r="T2" t="inlineStr">
+        <is>
+          <t>0.7268822843822844 ∓ 0.03697914334277689</t>
+        </is>
+      </c>
+      <c r="U2" t="inlineStr">
+        <is>
+          <t>0.7572912457351817 ∓ 0.033005034864855266</t>
+        </is>
+      </c>
+      <c r="V2" t="inlineStr">
+        <is>
+          <t>0.7341394025604553 ∓ 0.031950041839222024</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="n">
+        <v>1.109490740740741e-07</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>SVC_VertexHistogram_precomputed</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="D3" s="2" t="n">
+        <v>3.1084375e-06</v>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>{'C': 0.1, 'class_weight': None, 'kernel_type': 'precomputed'}</t>
+        </is>
+      </c>
+      <c r="F3" t="n">
+        <v>0.86</v>
+      </c>
+      <c r="G3" s="2" t="n">
+        <v>1.104976851851852e-07</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0.06385964912280706</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0.06508501816854229</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0.07885986562457159</v>
+      </c>
+      <c r="K3" t="n">
+        <v>0.7894736842105263</v>
+      </c>
+      <c r="L3" t="n">
+        <v>0.7838029416976786</v>
+      </c>
+      <c r="M3" t="n">
+        <v>0.7339743589743589</v>
+      </c>
+      <c r="N3" t="n">
+        <v>0.8533333333333334</v>
+      </c>
+      <c r="O3" t="n">
+        <v>0.8488879598662209</v>
+      </c>
+      <c r="P3" t="n">
+        <v>0.8128342245989305</v>
+      </c>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">              precision    recall  f1-score   support
+          -1       0.70      0.58      0.64        12
+           1       0.82      0.88      0.85        26
+    accuracy                           0.79        38
+   macro avg       0.76      0.73      0.74        38
+weighted avg       0.78      0.79      0.78        38
+</t>
+        </is>
+      </c>
+      <c r="R3" t="inlineStr">
+        <is>
+          <t>0.8509246088193457 ∓ 0.04830663543774094</t>
+        </is>
+      </c>
+      <c r="S3" t="inlineStr">
+        <is>
+          <t>0.8467074324031273 ∓ 0.05005363356539167</t>
+        </is>
+      </c>
+      <c r="T3" t="inlineStr">
+        <is>
+          <t>0.8108974358974358 ∓ 0.06698085453717943</t>
+        </is>
+      </c>
+      <c r="U3" t="inlineStr">
+        <is>
+          <t>0.8528665354690762 ∓ 0.05450402199834391</t>
+        </is>
+      </c>
+      <c r="V3" t="inlineStr">
+        <is>
+          <t>0.8509246088193457 ∓ 0.04830663543774094</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="n">
+        <v>1.046527777777778e-07</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>SVC_EdgeHistogram_precomputed</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="D4" s="2" t="n">
+        <v>2.622118055555556e-06</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>{'C': 0.1, 'class_weight': 'balanced', 'kernel_type': 'precomputed'}</t>
+        </is>
+      </c>
+      <c r="F4" t="n">
+        <v>0.8666666666666668</v>
+      </c>
+      <c r="G4" s="2" t="n">
+        <v>1.11412037037037e-07</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0.09052631578947368</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0.08571898496240593</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0.0792883587001233</v>
+      </c>
+      <c r="K4" t="n">
+        <v>0.7894736842105263</v>
+      </c>
+      <c r="L4" t="n">
+        <v>0.7957393483709274</v>
+      </c>
+      <c r="M4" t="n">
+        <v>0.8012820512820513</v>
+      </c>
+      <c r="N4" t="n">
+        <v>0.88</v>
+      </c>
+      <c r="O4" t="n">
+        <v>0.8814583333333333</v>
+      </c>
+      <c r="P4" t="n">
+        <v>0.8805704099821746</v>
+      </c>
+      <c r="Q4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">              precision    recall  f1-score   support
+          -1       0.62      0.83      0.71        12
+           1       0.91      0.77      0.83        26
+    accuracy                           0.79        38
+   macro avg       0.77      0.80      0.77        38
+weighted avg       0.82      0.79      0.80        38
+</t>
+        </is>
+      </c>
+      <c r="R4" t="inlineStr">
+        <is>
+          <t>0.8402560455192034 ∓ 0.07126773648490294</t>
+        </is>
+      </c>
+      <c r="S4" t="inlineStr">
+        <is>
+          <t>0.845150629585242 ∓ 0.06769809702714208</t>
+        </is>
+      </c>
+      <c r="T4" t="inlineStr">
+        <is>
+          <t>0.8527663170163169 ∓ 0.06229265265859301</t>
+        </is>
+      </c>
+      <c r="U4" t="inlineStr">
+        <is>
+          <t>0.8668971531355432 ∓ 0.052333965797823095</t>
+        </is>
+      </c>
+      <c r="V4" t="inlineStr">
+        <is>
+          <t>0.8402560455192034 ∓ 0.07126773648490294</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="n">
+        <v>1.242824074074074e-07</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>SVC_CombinedHistogram_precomputed</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="D5" s="2" t="n">
+        <v>5.399120370370371e-06</v>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>{'C': 0.5, 'class_weight': None, 'kernel_type': 'precomputed', 'weights': [1, 1]}</t>
+        </is>
+      </c>
+      <c r="F5" t="n">
+        <v>0.8866666666666667</v>
+      </c>
+      <c r="G5" s="2" t="n">
+        <v>1.210300925925926e-07</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0.1435087719298245</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0.1406272445820433</v>
+      </c>
+      <c r="J5" t="n">
+        <v>0.1540861099684629</v>
+      </c>
+      <c r="K5" t="n">
+        <v>0.7631578947368421</v>
+      </c>
+      <c r="L5" t="n">
+        <v>0.7655727554179567</v>
+      </c>
+      <c r="M5" t="n">
+        <v>0.7371794871794872</v>
+      </c>
+      <c r="N5" t="n">
+        <v>0.9066666666666666</v>
+      </c>
+      <c r="O5" t="n">
+        <v>0.9062</v>
+      </c>
+      <c r="P5" t="n">
+        <v>0.8912655971479502</v>
+      </c>
+      <c r="Q5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">              precision    recall  f1-score   support
+          -1       0.62      0.67      0.64        12
+           1       0.84      0.81      0.82        26
+    accuracy                           0.76        38
+   macro avg       0.73      0.74      0.73        38
+weighted avg       0.77      0.76      0.77        38
+</t>
+        </is>
+      </c>
+      <c r="R5" t="inlineStr">
+        <is>
+          <t>0.8509246088193457 ∓ 0.05643424351194077</t>
+        </is>
+      </c>
+      <c r="S5" t="inlineStr">
+        <is>
+          <t>0.8486017604628454 ∓ 0.056450636111349616</t>
+        </is>
+      </c>
+      <c r="T5" t="inlineStr">
+        <is>
+          <t>0.8177884615384615 ∓ 0.07016532164910769</t>
+        </is>
+      </c>
+      <c r="U5" t="inlineStr">
+        <is>
+          <t>0.8545790860763637 ∓ 0.05942134049115665</t>
+        </is>
+      </c>
+      <c r="V5" t="inlineStr">
+        <is>
+          <t>0.8509246088193457 ∓ 0.05643424351194077</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="n">
+        <v>6.475694444444445e-08</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>SVC_NX_combined_Histogram_rbf</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="D6" s="2" t="n">
+        <v>0.01246266328703704</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>{'C': 0.75, 'Histogram_Type': 'node+1', 'class_weight': None, 'kernel_type': 'poly'}</t>
+        </is>
+      </c>
+      <c r="F6" t="n">
+        <v>0.9066666666666666</v>
+      </c>
+      <c r="G6" s="2" t="n">
+        <v>5.540509259259259e-08</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0.08421052631578951</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0.08027504659083617</v>
+      </c>
+      <c r="J6" t="n">
+        <v>0.07520910462086938</v>
+      </c>
+      <c r="K6" t="n">
+        <v>0.8157894736842105</v>
+      </c>
+      <c r="L6" t="n">
+        <v>0.8203842940685045</v>
+      </c>
+      <c r="M6" t="n">
+        <v>0.8205128205128205</v>
+      </c>
+      <c r="N6" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="O6" t="n">
+        <v>0.9006593406593407</v>
+      </c>
+      <c r="P6" t="n">
+        <v>0.8957219251336899</v>
+      </c>
+      <c r="Q6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">              precision    recall  f1-score   support
+          -1       0.67      0.83      0.74        12
+           1       0.91      0.81      0.86        26
+    accuracy                           0.82        38
+   macro avg       0.79      0.82      0.80        38
+weighted avg       0.84      0.82      0.82        38
+</t>
+        </is>
+      </c>
+      <c r="R6" t="inlineStr">
+        <is>
+          <t>0.8934566145092461 ∓ 0.05738459834975402</t>
+        </is>
+      </c>
+      <c r="S6" t="inlineStr">
+        <is>
+          <t>0.8947380127840485 ∓ 0.05587865319234957</t>
+        </is>
+      </c>
+      <c r="T6" t="inlineStr">
+        <is>
+          <t>0.8862907925407926 ∓ 0.06122524780442136</t>
+        </is>
+      </c>
+      <c r="U6" t="inlineStr">
+        <is>
+          <t>0.9008044880447628 ∓ 0.05389213161855249</t>
+        </is>
+      </c>
+      <c r="V6" t="inlineStr">
+        <is>
+          <t>0.8934566145092461 ∓ 0.05738459834975402</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="2" t="n">
+        <v>1.621527777777778e-08</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Blind_Classifier</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="D7" s="2" t="n">
+        <v>4.731828703703704e-07</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="F7" t="n">
+        <v>0.5800000000000001</v>
+      </c>
+      <c r="G7" s="2" t="n">
+        <v>1.140046296296296e-08</v>
+      </c>
+      <c r="H7" t="n">
+        <v>-0.02421052631578946</v>
+      </c>
+      <c r="I7" t="n">
+        <v>-0.03110177552314519</v>
+      </c>
+      <c r="J7" t="n">
+        <v>0</v>
+      </c>
+      <c r="K7" t="n">
+        <v>0.6842105263157895</v>
+      </c>
+      <c r="L7" t="n">
+        <v>0.555921052631579</v>
+      </c>
+      <c r="M7" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="N7" t="n">
+        <v>0.66</v>
+      </c>
+      <c r="O7" t="n">
+        <v>0.5248192771084338</v>
+      </c>
+      <c r="P7" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="Q7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">              precision    recall  f1-score   support
+          -1       0.00      0.00      0.00        12
+           1       0.68      1.00      0.81        26
+    accuracy                           0.68        38
+   macro avg       0.34      0.50      0.41        38
+weighted avg       0.47      0.68      0.56        38
+</t>
+        </is>
+      </c>
+      <c r="R7" t="inlineStr">
+        <is>
+          <t>0.43271692745376955 ∓ 0.1411590572584785</t>
+        </is>
+      </c>
+      <c r="S7" t="inlineStr">
+        <is>
+          <t>0.33519567246799 ∓ 0.15493108617803367</t>
+        </is>
+      </c>
+      <c r="T7" t="inlineStr">
+        <is>
+          <t>0.45034965034965035 ∓ 0.0431832769767607</t>
+        </is>
+      </c>
+      <c r="U7" t="inlineStr">
+        <is>
+          <t>0.32539934387609765 ∓ 0.1525110108203507</t>
+        </is>
+      </c>
+      <c r="V7" t="inlineStr">
+        <is>
+          <t>0.43271692745376955 ∓ 0.1411590572584785</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="2" t="n">
+        <v>8.391203703703704e-09</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>RandomGuesser_uniform</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="D8" s="2" t="n">
+        <v>1.783912037037037e-06</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>{'strategy': 'most_frequent'}</t>
+        </is>
+      </c>
+      <c r="F8" t="n">
+        <v>0.6599999999999999</v>
+      </c>
+      <c r="G8" s="2" t="n">
+        <v>1.417824074074074e-08</v>
+      </c>
+      <c r="H8" t="n">
+        <v>-0.02421052631578946</v>
+      </c>
+      <c r="I8" t="n">
+        <v>-0.03110177552314519</v>
+      </c>
+      <c r="J8" t="n">
+        <v>0</v>
+      </c>
+      <c r="K8" t="n">
+        <v>0.6842105263157895</v>
+      </c>
+      <c r="L8" t="n">
+        <v>0.555921052631579</v>
+      </c>
+      <c r="M8" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="N8" t="n">
+        <v>0.66</v>
+      </c>
+      <c r="O8" t="n">
+        <v>0.5248192771084338</v>
+      </c>
+      <c r="P8" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="Q8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">              precision    recall  f1-score   support
+          -1       0.00      0.00      0.00        12
+           1       0.68      1.00      0.81        26
+    accuracy                           0.68        38
+   macro avg       0.34      0.50      0.41        38
+weighted avg       0.47      0.68      0.56        38
+</t>
+        </is>
+      </c>
+      <c r="R8" t="inlineStr">
+        <is>
+          <t>0.6651493598862019 ∓ 0.0385639962422283</t>
+        </is>
+      </c>
+      <c r="S8" t="inlineStr">
+        <is>
+          <t>0.532262365445727 ∓ 0.048261888836995046</t>
+        </is>
+      </c>
+      <c r="T8" t="inlineStr">
+        <is>
+          <t>0.5 ∓ 0.0</t>
+        </is>
+      </c>
+      <c r="U8" t="inlineStr">
+        <is>
+          <t>0.44435937022595706 ∓ 0.04902786144463162</t>
+        </is>
+      </c>
+      <c r="V8" t="inlineStr">
+        <is>
+          <t>0.6651493598862019 ∓ 0.0385639962422283</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="2" t="n">
+        <v>2.730555555555555e-07</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>(7)-NN_Classifier_GED</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="D9" s="2" t="n">
+        <v>0.0003391966898148148</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>{'comparison_method': 'LowerBound-Distance', 'metric': 'euclidean', 'n_neighbors': 1, 'weights': 'uniform'}</t>
+        </is>
+      </c>
+      <c r="F9" t="n">
+        <v>0.8933333333333333</v>
+      </c>
+      <c r="G9" s="2" t="n">
+        <v>1.493171296296296e-07</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0.124561403508772</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0.1197808909806234</v>
+      </c>
+      <c r="J9" t="n">
+        <v>0.09830773801362036</v>
+      </c>
+      <c r="K9" t="n">
+        <v>0.8421052631578947</v>
+      </c>
+      <c r="L9" t="n">
+        <v>0.8468045112781956</v>
+      </c>
+      <c r="M9" t="n">
+        <v>0.8621794871794871</v>
+      </c>
+      <c r="N9" t="n">
+        <v>0.9666666666666667</v>
+      </c>
+      <c r="O9" t="n">
+        <v>0.9665854022588189</v>
+      </c>
+      <c r="P9" t="n">
+        <v>0.9604872251931075</v>
+      </c>
+      <c r="Q9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">              precision    recall  f1-score   support
+          -1       0.69      0.92      0.79        12
+           1       0.95      0.81      0.88        26
+    accuracy                           0.84        38
+   macro avg       0.82      0.86      0.83        38
+weighted avg       0.87      0.84      0.85        38
+</t>
+        </is>
+      </c>
+      <c r="R9" t="inlineStr">
+        <is>
+          <t>0.8880512091038406 ∓ 0.04986172525160431</t>
+        </is>
+      </c>
+      <c r="S9" t="inlineStr">
+        <is>
+          <t>0.8892953342985986 ∓ 0.048061377771183876</t>
+        </is>
+      </c>
+      <c r="T9" t="inlineStr">
+        <is>
+          <t>0.8787861305361305 ∓ 0.044097984266033105</t>
+        </is>
+      </c>
+      <c r="U9" t="inlineStr">
+        <is>
+          <t>0.896456540328394 ∓ 0.04504686643777451</t>
+        </is>
+      </c>
+      <c r="V9" t="inlineStr">
+        <is>
+          <t>0.8880512091038406 ∓ 0.04986172525160431</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="2" t="n">
+        <v>2.999421296296296e-07</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>SVC_Base-GED_precomputed</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>GEDLIB_Calculator</t>
+        </is>
+      </c>
+      <c r="D10" s="2" t="n">
+        <v>7.667263888888888e-05</v>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>{'C': 0.75, 'class_weight': 'balanced', 'kernel_type': 'precomputed'}</t>
+        </is>
+      </c>
+      <c r="F10" t="n">
+        <v>0.8933333333333333</v>
+      </c>
+      <c r="G10" s="2" t="n">
+        <v>2.68287037037037e-07</v>
+      </c>
+      <c r="H10" t="n">
+        <v>0.1905263157894737</v>
+      </c>
+      <c r="I10" t="n">
+        <v>0.1867715442452285</v>
+      </c>
+      <c r="J10" t="n">
+        <v>0.206002331002331</v>
+      </c>
+      <c r="K10" t="n">
+        <v>0.7894736842105263</v>
+      </c>
+      <c r="L10" t="n">
+        <v>0.7933603238866397</v>
+      </c>
+      <c r="M10" t="n">
+        <v>0.7788461538461539</v>
+      </c>
+      <c r="N10" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="O10" t="n">
+        <v>0.9801318681318681</v>
+      </c>
+      <c r="P10" t="n">
+        <v>0.9848484848484849</v>
+      </c>
+      <c r="Q10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">              precision    recall  f1-score   support
+          -1       0.64      0.75      0.69        12
+           1       0.88      0.81      0.84        26
+    accuracy                           0.79        38
+   macro avg       0.76      0.78      0.77        38
+weighted avg       0.80      0.79      0.79        38
+</t>
+        </is>
+      </c>
+      <c r="R10" t="inlineStr">
+        <is>
+          <t>0.8617354196301565 ∓ 0.0451442543530954</t>
+        </is>
+      </c>
+      <c r="S10" t="inlineStr">
+        <is>
+          <t>0.8610253672739748 ∓ 0.043881725613342505</t>
+        </is>
+      </c>
+      <c r="T10" t="inlineStr">
+        <is>
+          <t>0.8352127039627039 ∓ 0.047244450184508215</t>
+        </is>
+      </c>
+      <c r="U10" t="inlineStr">
+        <is>
+          <t>0.8656595693437799 ∓ 0.04515172033072602</t>
+        </is>
+      </c>
+      <c r="V10" t="inlineStr">
+        <is>
+          <t>0.8617354196301565 ∓ 0.0451442543530954</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="2" t="n">
+        <v>2.606828703703704e-07</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>SVC_Diffusion-GED_precomputed</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>GEDLIB_Calculator</t>
+        </is>
+      </c>
+      <c r="D11" s="2" t="n">
+        <v>0.001372016875</v>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>{'C': 0.1, 'KERNEL_diffusion_function': 'exp_diff_kernel', 'KERNEL_iteration_t': 5, 'KERNEL_llambda': 0.1, 'class_weight': None, 'kernel_type': 'precomputed'}</t>
+        </is>
+      </c>
+      <c r="F11" t="n">
+        <v>0.8533333333333335</v>
+      </c>
+      <c r="G11" s="2" t="n">
+        <v>2.309375e-07</v>
+      </c>
+      <c r="H11" t="n">
+        <v>0.1842105263157895</v>
+      </c>
+      <c r="I11" t="n">
+        <v>0.1823323013415892</v>
+      </c>
+      <c r="J11" t="n">
+        <v>0.201923076923077</v>
+      </c>
+      <c r="K11" t="n">
+        <v>0.8157894736842105</v>
+      </c>
+      <c r="L11" t="n">
+        <v>0.8176676986584108</v>
+      </c>
+      <c r="M11" t="n">
+        <v>0.798076923076923</v>
+      </c>
+      <c r="N11" t="n">
+        <v>1</v>
+      </c>
+      <c r="O11" t="n">
+        <v>1</v>
+      </c>
+      <c r="P11" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">              precision    recall  f1-score   support
+          -1       0.69      0.75      0.72        12
+           1       0.88      0.85      0.86        26
+    accuracy                           0.82        38
+   macro avg       0.79      0.80      0.79        38
+weighted avg       0.82      0.82      0.82        38
+</t>
+        </is>
+      </c>
+      <c r="R11" t="inlineStr">
+        <is>
+          <t>0.8671408250355619 ∓ 0.032655085739429046</t>
+        </is>
+      </c>
+      <c r="S11" t="inlineStr">
+        <is>
+          <t>0.8652135349275365 ∓ 0.03234707238123895</t>
+        </is>
+      </c>
+      <c r="T11" t="inlineStr">
+        <is>
+          <t>0.8365011655011655 ∓ 0.03706432214818053</t>
+        </is>
+      </c>
+      <c r="U11" t="inlineStr">
+        <is>
+          <t>0.8685820072135861 ∓ 0.03222465489608996</t>
+        </is>
+      </c>
+      <c r="V11" t="inlineStr">
+        <is>
+          <t>0.8671408250355619 ∓ 0.032655085739429046</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="2" t="n">
+        <v>2.901736111111111e-07</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>SVC_Trivial-GED_precomputed</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>GEDLIB_Calculator</t>
+        </is>
+      </c>
+      <c r="D12" s="2" t="n">
+        <v>0.0003861859490740741</v>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>{'C': 0.5, 'KERNEL_similarity_function': 'k1', 'class_weight': 'balanced', 'kernel_type': 'precomputed'}</t>
+        </is>
+      </c>
+      <c r="F12" t="n">
+        <v>0.8333333333333334</v>
+      </c>
+      <c r="G12" s="2" t="n">
+        <v>2.636805555555556e-07</v>
+      </c>
+      <c r="H12" t="n">
+        <v>0.07614035087719295</v>
+      </c>
+      <c r="I12" t="n">
+        <v>0.07043330998074782</v>
+      </c>
+      <c r="J12" t="n">
+        <v>0.06494241053064587</v>
+      </c>
+      <c r="K12" t="n">
+        <v>0.7105263157894737</v>
+      </c>
+      <c r="L12" t="n">
+        <v>0.7200834073444802</v>
+      </c>
+      <c r="M12" t="n">
+        <v>0.7211538461538461</v>
+      </c>
+      <c r="N12" t="n">
+        <v>0.7866666666666666</v>
+      </c>
+      <c r="O12" t="n">
+        <v>0.790516717325228</v>
+      </c>
+      <c r="P12" t="n">
+        <v>0.786096256684492</v>
+      </c>
+      <c r="Q12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">              precision    recall  f1-score   support
+          -1       0.53      0.75      0.62        12
+           1       0.86      0.69      0.77        26
+    accuracy                           0.71        38
+   macro avg       0.69      0.72      0.69        38
+weighted avg       0.75      0.71      0.72        38
+</t>
+        </is>
+      </c>
+      <c r="R12" t="inlineStr">
+        <is>
+          <t>0.7763869132290184 ∓ 0.060889051454919164</t>
+        </is>
+      </c>
+      <c r="S12" t="inlineStr">
+        <is>
+          <t>0.7820991897894939 ∓ 0.05706002704581839</t>
+        </is>
+      </c>
+      <c r="T12" t="inlineStr">
+        <is>
+          <t>0.7841975524475525 ∓ 0.06252923761260223</t>
+        </is>
+      </c>
+      <c r="U12" t="inlineStr">
+        <is>
+          <t>0.8096890081475383 ∓ 0.04947202264759567</t>
+        </is>
+      </c>
+      <c r="V12" t="inlineStr">
+        <is>
+          <t>0.7763869132290184 ∓ 0.060889051454919164</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="2" t="n">
+        <v>4.545138888888889e-08</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>SVC_Simple_Prototype_GED_poly</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>GEDLIB_Calculator</t>
+        </is>
+      </c>
+      <c r="D13" s="2" t="n">
+        <v>0.003425477928240741</v>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>{'KERNEL_classwise': False, 'KERNEL_prototype_size': 1, 'KERNEL_selection_method': 'RPS', 'KERNEL_single_class': False, 'kernel_type': 'rbf'}</t>
+        </is>
+      </c>
+      <c r="F13" t="n">
+        <v>0.8866666666666667</v>
+      </c>
+      <c r="G13" s="2" t="n">
+        <v>7.310185185185185e-08</v>
+      </c>
+      <c r="H13" t="n">
+        <v>0.1498245614035089</v>
+      </c>
+      <c r="I13" t="n">
+        <v>0.1489531608306157</v>
+      </c>
+      <c r="J13" t="n">
+        <v>0.1710944284473697</v>
+      </c>
+      <c r="K13" t="n">
+        <v>0.7368421052631579</v>
+      </c>
+      <c r="L13" t="n">
+        <v>0.7368421052631579</v>
+      </c>
+      <c r="M13" t="n">
+        <v>0.6955128205128205</v>
+      </c>
+      <c r="N13" t="n">
+        <v>0.8866666666666667</v>
+      </c>
+      <c r="O13" t="n">
+        <v>0.8857952660937736</v>
+      </c>
+      <c r="P13" t="n">
+        <v>0.8666072489601901</v>
+      </c>
+      <c r="Q13" t="inlineStr">
+        <is>
+          <t xml:space="preserve">              precision    recall  f1-score   support
+          -1       0.58      0.58      0.58        12
+           1       0.81      0.81      0.81        26
+    accuracy                           0.74        38
+   macro avg       0.70      0.70      0.70        38
+weighted avg       0.74      0.74      0.74        38
+</t>
+        </is>
+      </c>
+      <c r="R13" t="inlineStr">
+        <is>
+          <t>0.8349928876244667 ∓ 0.054323805762157146</t>
+        </is>
+      </c>
+      <c r="S13" t="inlineStr">
+        <is>
+          <t>0.8334393761279628 ∓ 0.053504530433513324</t>
+        </is>
+      </c>
+      <c r="T13" t="inlineStr">
+        <is>
+          <t>0.8017628205128204 ∓ 0.06363430116594176</t>
+        </is>
+      </c>
+      <c r="U13" t="inlineStr">
+        <is>
+          <t>0.8393536373772308 ∓ 0.05785490679884687</t>
+        </is>
+      </c>
+      <c r="V13" t="inlineStr">
+        <is>
+          <t>0.8349928876244667 ∓ 0.054323805762157146</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="2" t="n">
+        <v>4.795509259259259e-06</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>SVC_Zero-GED_precomputed</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>GEDLIB_Calculator</t>
+        </is>
+      </c>
+      <c r="D14" s="2" t="n">
+        <v>0.00756443986111111</v>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>{'C': 0.25, 'KERNEL_I_size': 1, 'KERNEL_aggregation_method': 'sum', 'KERNEL_selection_method': 'RPS', 'KERNEL_single_class': True, 'class_weight': 'balanced', 'kernel_type': 'precomputed'}</t>
+        </is>
+      </c>
+      <c r="F14" t="n">
+        <v>0.8333333333333334</v>
+      </c>
+      <c r="G14" s="2" t="n">
+        <v>4.374756944444445e-06</v>
+      </c>
+      <c r="H14" t="n">
+        <v>0.07614035087719295</v>
+      </c>
+      <c r="I14" t="n">
+        <v>0.07043330998074782</v>
+      </c>
+      <c r="J14" t="n">
+        <v>0.06494241053064587</v>
+      </c>
+      <c r="K14" t="n">
+        <v>0.7105263157894737</v>
+      </c>
+      <c r="L14" t="n">
+        <v>0.7200834073444802</v>
+      </c>
+      <c r="M14" t="n">
+        <v>0.7211538461538461</v>
+      </c>
+      <c r="N14" t="n">
+        <v>0.7866666666666666</v>
+      </c>
+      <c r="O14" t="n">
+        <v>0.790516717325228</v>
+      </c>
+      <c r="P14" t="n">
+        <v>0.786096256684492</v>
+      </c>
+      <c r="Q14" t="inlineStr">
+        <is>
+          <t xml:space="preserve">              precision    recall  f1-score   support
+          -1       0.53      0.75      0.62        12
+           1       0.86      0.69      0.77        26
+    accuracy                           0.71        38
+   macro avg       0.69      0.72      0.69        38
+weighted avg       0.75      0.71      0.72        38
+</t>
+        </is>
+      </c>
+      <c r="R14" t="inlineStr">
+        <is>
+          <t>0.7712660028449502 ∓ 0.06673822081133857</t>
+        </is>
+      </c>
+      <c r="S14" t="inlineStr">
+        <is>
+          <t>0.777171841945989 ∓ 0.06284769140623572</t>
+        </is>
+      </c>
+      <c r="T14" t="inlineStr">
+        <is>
+          <t>0.7838916083916083 ∓ 0.05554880603296297</t>
+        </is>
+      </c>
+      <c r="U14" t="inlineStr">
+        <is>
+          <t>0.8094791297268078 ∓ 0.04107948027281789</t>
+        </is>
+      </c>
+      <c r="V14" t="inlineStr">
+        <is>
+          <t>0.7712660028449502 ∓ 0.06673822081133857</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="2" t="n">
+        <v>4.505942129629629e-05</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>SVC_Random-Walk-Edit_precomputed</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>GEDLIB_Calculator</t>
+        </is>
+      </c>
+      <c r="D15" s="2" t="n">
+        <v>0.0007785123379629629</v>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>{'C': 0.1, 'KERNEL_decay_lambda': 0.01, 'KERNEL_max_walk_length': 5, 'class_weight': 'balanced', 'kernel_type': 'precomputed'}</t>
+        </is>
+      </c>
+      <c r="F15" t="n">
+        <v>0.8533333333333333</v>
+      </c>
+      <c r="G15" s="2" t="n">
+        <v>4.84565625e-05</v>
+      </c>
+      <c r="H15" t="n">
+        <v>0.09052631578947368</v>
+      </c>
+      <c r="I15" t="n">
+        <v>0.08609797220323523</v>
+      </c>
+      <c r="J15" t="n">
+        <v>0.08404177521824574</v>
+      </c>
+      <c r="K15" t="n">
+        <v>0.7894736842105263</v>
+      </c>
+      <c r="L15" t="n">
+        <v>0.7957393483709274</v>
+      </c>
+      <c r="M15" t="n">
+        <v>0.8012820512820513</v>
+      </c>
+      <c r="N15" t="n">
+        <v>0.88</v>
+      </c>
+      <c r="O15" t="n">
+        <v>0.8818373205741626</v>
+      </c>
+      <c r="P15" t="n">
+        <v>0.8853238265002971</v>
+      </c>
+      <c r="Q15" t="inlineStr">
+        <is>
+          <t xml:space="preserve">              precision    recall  f1-score   support
+          -1       0.62      0.83      0.71        12
+           1       0.91      0.77      0.83        26
+    accuracy                           0.79        38
+   macro avg       0.77      0.80      0.77        38
+weighted avg       0.82      0.79      0.80        38
+</t>
+        </is>
+      </c>
+      <c r="R15" t="inlineStr">
+        <is>
+          <t>0.845945945945946 ∓ 0.06306502786509129</t>
+        </is>
+      </c>
+      <c r="S15" t="inlineStr">
+        <is>
+          <t>0.8498975828008086 ∓ 0.06011629825235554</t>
+        </is>
+      </c>
+      <c r="T15" t="inlineStr">
+        <is>
+          <t>0.8498752913752913 ∓ 0.05531692661695446</t>
+        </is>
+      </c>
+      <c r="U15" t="inlineStr">
+        <is>
+          <t>0.8646975038279384 ∓ 0.04989484530983184</t>
+        </is>
+      </c>
+      <c r="V15" t="inlineStr">
+        <is>
+          <t>0.845945945945946 ∓ 0.06306502786509129</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="2" t="n">
+        <v>2.606365740740741e-07</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>(7)-NN_Classifier_GED</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="D16" s="2" t="n">
+        <v>1.832678240740741e-05</v>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>{'comparison_method': 'UpperBound-Distance', 'metric': 'euclidean', 'n_neighbors': 1, 'weights': 'uniform'}</t>
+        </is>
+      </c>
+      <c r="F16" t="n">
+        <v>0.8533333333333335</v>
+      </c>
+      <c r="G16" s="2" t="n">
+        <v>1.552199074074074e-07</v>
+      </c>
+      <c r="H16" t="n">
+        <v>0.08385964912280697</v>
+      </c>
+      <c r="I16" t="n">
+        <v>0.07891272658912285</v>
+      </c>
+      <c r="J16" t="n">
+        <v>0.06948443713149599</v>
+      </c>
+      <c r="K16" t="n">
+        <v>0.7894736842105263</v>
+      </c>
+      <c r="L16" t="n">
+        <v>0.7957393483709274</v>
+      </c>
+      <c r="M16" t="n">
+        <v>0.8012820512820513</v>
+      </c>
+      <c r="N16" t="n">
+        <v>0.8733333333333333</v>
+      </c>
+      <c r="O16" t="n">
+        <v>0.8746520749600503</v>
+      </c>
+      <c r="P16" t="n">
+        <v>0.8707664884135473</v>
+      </c>
+      <c r="Q16" t="inlineStr">
+        <is>
+          <t xml:space="preserve">              precision    recall  f1-score   support
+          -1       0.62      0.83      0.71        12
+           1       0.91      0.77      0.83        26
+    accuracy                           0.79        38
+   macro avg       0.77      0.80      0.77        38
+weighted avg       0.82      0.79      0.80        38
+</t>
+        </is>
+      </c>
+      <c r="R16" t="inlineStr">
+        <is>
+          <t>0.8408250355618776 ∓ 0.056060849548073145</t>
+        </is>
+      </c>
+      <c r="S16" t="inlineStr">
+        <is>
+          <t>0.8418955492141654 ∓ 0.05370967815016412</t>
+        </is>
+      </c>
+      <c r="T16" t="inlineStr">
+        <is>
+          <t>0.8232144522144521 ∓ 0.05468743613897573</t>
+        </is>
+      </c>
+      <c r="U16" t="inlineStr">
+        <is>
+          <t>0.8506353542966816 ∓ 0.053531484312804474</t>
+        </is>
+      </c>
+      <c r="V16" t="inlineStr">
+        <is>
+          <t>0.8408250355618776 ∓ 0.056060849548073145</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="2" t="n">
+        <v>2.955092592592593e-07</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>SVC_Base-GED_precomputed</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Dummy_Calculator</t>
+        </is>
+      </c>
+      <c r="D17" s="2" t="n">
+        <v>6.421006944444445e-06</v>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>{'C': 0.5, 'class_weight': None, 'kernel_type': 'precomputed'}</t>
+        </is>
+      </c>
+      <c r="F17" t="n">
+        <v>0.8866666666666667</v>
+      </c>
+      <c r="G17" s="2" t="n">
+        <v>2.789351851851852e-07</v>
+      </c>
+      <c r="H17" t="n">
+        <v>0.08421052631578951</v>
+      </c>
+      <c r="I17" t="n">
+        <v>0.07984733571810021</v>
+      </c>
+      <c r="J17" t="n">
+        <v>0.07045568810274694</v>
+      </c>
+      <c r="K17" t="n">
+        <v>0.8157894736842105</v>
+      </c>
+      <c r="L17" t="n">
+        <v>0.8203842940685045</v>
+      </c>
+      <c r="M17" t="n">
+        <v>0.8205128205128205</v>
+      </c>
+      <c r="N17" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="O17" t="n">
+        <v>0.9002316297866048</v>
+      </c>
+      <c r="P17" t="n">
+        <v>0.8909685086155674</v>
+      </c>
+      <c r="Q17" t="inlineStr">
+        <is>
+          <t xml:space="preserve">              precision    recall  f1-score   support
+          -1       0.67      0.83      0.74        12
+           1       0.91      0.81      0.86        26
+    accuracy                           0.82        38
+   macro avg       0.79      0.82      0.80        38
+weighted avg       0.84      0.82      0.82        38
+</t>
+        </is>
+      </c>
+      <c r="R17" t="inlineStr">
+        <is>
+          <t>0.835135135135135 ∓ 0.03443016300935652</t>
+        </is>
+      </c>
+      <c r="S17" t="inlineStr">
+        <is>
+          <t>0.8340264376932716 ∓ 0.033275475071983265</t>
+        </is>
+      </c>
+      <c r="T17" t="inlineStr">
+        <is>
+          <t>0.8128205128205128 ∓ 0.04383690119606617</t>
+        </is>
+      </c>
+      <c r="U17" t="inlineStr">
+        <is>
+          <t>0.8496810200377674 ∓ 0.03853898548580617</t>
+        </is>
+      </c>
+      <c r="V17" t="inlineStr">
+        <is>
+          <t>0.835135135135135 ∓ 0.03443016300935652</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="2" t="n">
+        <v>2.605439814814815e-07</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>SVC_Diffusion-GED_precomputed</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Dummy_Calculator</t>
+        </is>
+      </c>
+      <c r="D18" s="2" t="n">
+        <v>6.748608796296296e-05</v>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>{'C': 0.1, 'KERNEL_diffusion_function': 'exp_diff_kernel', 'KERNEL_iteration_t': 5, 'KERNEL_llambda': 0.1, 'class_weight': None, 'kernel_type': 'precomputed'}</t>
+        </is>
+      </c>
+      <c r="F18" t="n">
+        <v>0.8666666666666666</v>
+      </c>
+      <c r="G18" s="2" t="n">
+        <v>2.351851851851852e-07</v>
+      </c>
+      <c r="H18" t="n">
+        <v>0.1501754385964912</v>
+      </c>
+      <c r="I18" t="n">
+        <v>0.1475492904549724</v>
+      </c>
+      <c r="J18" t="n">
+        <v>0.1638900315370904</v>
+      </c>
+      <c r="K18" t="n">
+        <v>0.7631578947368421</v>
+      </c>
+      <c r="L18" t="n">
+        <v>0.7655727554179567</v>
+      </c>
+      <c r="M18" t="n">
+        <v>0.7371794871794872</v>
+      </c>
+      <c r="N18" t="n">
+        <v>0.9133333333333333</v>
+      </c>
+      <c r="O18" t="n">
+        <v>0.9131220458729291</v>
+      </c>
+      <c r="P18" t="n">
+        <v>0.9010695187165776</v>
+      </c>
+      <c r="Q18" t="inlineStr">
+        <is>
+          <t xml:space="preserve">              precision    recall  f1-score   support
+          -1       0.62      0.67      0.64        12
+           1       0.84      0.81      0.82        26
+    accuracy                           0.76        38
+   macro avg       0.73      0.74      0.73        38
+weighted avg       0.77      0.76      0.77        38
+</t>
+        </is>
+      </c>
+      <c r="R18" t="inlineStr">
+        <is>
+          <t>0.8297297297297298 ∓ 0.050527605943799736</t>
+        </is>
+      </c>
+      <c r="S18" t="inlineStr">
+        <is>
+          <t>0.8302245513700643 ∓ 0.04767172306235809</t>
+        </is>
+      </c>
+      <c r="T18" t="inlineStr">
+        <is>
+          <t>0.8084772727272729 ∓ 0.04863219590213387</t>
+        </is>
+      </c>
+      <c r="U18" t="inlineStr">
+        <is>
+          <t>0.8402477161470296 ∓ 0.0475345739399581</t>
+        </is>
+      </c>
+      <c r="V18" t="inlineStr">
+        <is>
+          <t>0.8297297297297298 ∓ 0.050527605943799736</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="2" t="n">
+        <v>2.963773148148148e-07</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>SVC_Trivial-GED_precomputed</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Dummy_Calculator</t>
+        </is>
+      </c>
+      <c r="D19" s="2" t="n">
+        <v>2.057517361111111e-05</v>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>{'C': 0.5, 'KERNEL_similarity_function': 'k1', 'class_weight': None, 'kernel_type': 'precomputed'}</t>
+        </is>
+      </c>
+      <c r="F19" t="n">
+        <v>0.8733333333333334</v>
+      </c>
+      <c r="G19" s="2" t="n">
+        <v>2.798611111111111e-07</v>
+      </c>
+      <c r="H19" t="n">
+        <v>0.05754385964912279</v>
+      </c>
+      <c r="I19" t="n">
+        <v>0.05730653611358871</v>
+      </c>
+      <c r="J19" t="n">
+        <v>0.0666049636637871</v>
+      </c>
+      <c r="K19" t="n">
+        <v>0.8157894736842105</v>
+      </c>
+      <c r="L19" t="n">
+        <v>0.8135227321790942</v>
+      </c>
+      <c r="M19" t="n">
+        <v>0.7756410256410258</v>
+      </c>
+      <c r="N19" t="n">
+        <v>0.8733333333333333</v>
+      </c>
+      <c r="O19" t="n">
+        <v>0.8708292682926829</v>
+      </c>
+      <c r="P19" t="n">
+        <v>0.8422459893048129</v>
+      </c>
+      <c r="Q19" t="inlineStr">
+        <is>
+          <t xml:space="preserve">              precision    recall  f1-score   support
+          -1       0.73      0.67      0.70        12
+           1       0.85      0.88      0.87        26
+    accuracy                           0.82        38
+   macro avg       0.79      0.78      0.78        38
+weighted avg       0.81      0.82      0.81        38
+</t>
+        </is>
+      </c>
+      <c r="R19" t="inlineStr">
+        <is>
+          <t>0.835135135135135 ∓ 0.03443016300935652</t>
+        </is>
+      </c>
+      <c r="S19" t="inlineStr">
+        <is>
+          <t>0.8323567322852476 ∓ 0.0338675480016161</t>
+        </is>
+      </c>
+      <c r="T19" t="inlineStr">
+        <is>
+          <t>0.7993589743589744 ∓ 0.04307408200111533</t>
+        </is>
+      </c>
+      <c r="U19" t="inlineStr">
+        <is>
+          <t>0.8409905475702051 ∓ 0.04041607478359179</t>
+        </is>
+      </c>
+      <c r="V19" t="inlineStr">
+        <is>
+          <t>0.835135135135135 ∓ 0.03443016300935652</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="2" t="n">
+        <v>3.678240740740741e-08</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>SVC_Simple_Prototype_GED_poly</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Dummy_Calculator</t>
+        </is>
+      </c>
+      <c r="D20" s="2" t="n">
+        <v>0.0001613113541666667</v>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>{'KERNEL_classwise': False, 'KERNEL_prototype_size': 1, 'KERNEL_selection_method': 'RPS', 'KERNEL_single_class': False, 'kernel_type': 'rbf'}</t>
+        </is>
+      </c>
+      <c r="F20" t="n">
+        <v>0.8800000000000001</v>
+      </c>
+      <c r="G20" s="2" t="n">
+        <v>2.892361111111111e-08</v>
+      </c>
+      <c r="H20" t="n">
+        <v>0.05719298245614035</v>
+      </c>
+      <c r="I20" t="n">
+        <v>0.05601402873987327</v>
+      </c>
+      <c r="J20" t="n">
+        <v>0.06563371269253604</v>
+      </c>
+      <c r="K20" t="n">
+        <v>0.7894736842105263</v>
+      </c>
+      <c r="L20" t="n">
+        <v>0.7894736842105263</v>
+      </c>
+      <c r="M20" t="n">
+        <v>0.7564102564102566</v>
+      </c>
+      <c r="N20" t="n">
+        <v>0.8466666666666667</v>
+      </c>
+      <c r="O20" t="n">
+        <v>0.8454877129503996</v>
+      </c>
+      <c r="P20" t="n">
+        <v>0.8220439691027926</v>
+      </c>
+      <c r="Q20" t="inlineStr">
+        <is>
+          <t xml:space="preserve">              precision    recall  f1-score   support
+          -1       0.67      0.67      0.67        12
+           1       0.85      0.85      0.85        26
+    accuracy                           0.79        38
+   macro avg       0.76      0.76      0.76        38
+weighted avg       0.79      0.79      0.79        38
+</t>
+        </is>
+      </c>
+      <c r="R20" t="inlineStr">
+        <is>
+          <t>0.8403982930298719 ∓ 0.04889837228382343</t>
+        </is>
+      </c>
+      <c r="S20" t="inlineStr">
+        <is>
+          <t>0.839768436882189 ∓ 0.04777417285931844</t>
+        </is>
+      </c>
+      <c r="T20" t="inlineStr">
+        <is>
+          <t>0.8169871794871794 ∓ 0.05610092848663261</t>
+        </is>
+      </c>
+      <c r="U20" t="inlineStr">
+        <is>
+          <t>0.8516852941322286 ∓ 0.04809713027475213</t>
+        </is>
+      </c>
+      <c r="V20" t="inlineStr">
+        <is>
+          <t>0.8403982930298719 ∓ 0.04889837228382343</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="2" t="n">
+        <v>4.814247685185186e-06</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>SVC_Zero-GED_precomputed</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Dummy_Calculator</t>
+        </is>
+      </c>
+      <c r="D21" s="2" t="n">
+        <v>0.002110413912037037</v>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>{'C': 0.5, 'KERNEL_I_size': 1, 'KERNEL_aggregation_method': 'sum', 'KERNEL_selection_method': 'RPS', 'KERNEL_single_class': False, 'class_weight': None, 'kernel_type': 'precomputed'}</t>
+        </is>
+      </c>
+      <c r="F21" t="n">
+        <v>0.8800000000000001</v>
+      </c>
+      <c r="G21" s="2" t="n">
+        <v>4.266493055555555e-06</v>
+      </c>
+      <c r="H21" t="n">
+        <v>0.05754385964912279</v>
+      </c>
+      <c r="I21" t="n">
+        <v>0.05730653611358871</v>
+      </c>
+      <c r="J21" t="n">
+        <v>0.0666049636637871</v>
+      </c>
+      <c r="K21" t="n">
+        <v>0.8157894736842105</v>
+      </c>
+      <c r="L21" t="n">
+        <v>0.8135227321790942</v>
+      </c>
+      <c r="M21" t="n">
+        <v>0.7756410256410258</v>
+      </c>
+      <c r="N21" t="n">
+        <v>0.8733333333333333</v>
+      </c>
+      <c r="O21" t="n">
+        <v>0.8708292682926829</v>
+      </c>
+      <c r="P21" t="n">
+        <v>0.8422459893048129</v>
+      </c>
+      <c r="Q21" t="inlineStr">
+        <is>
+          <t xml:space="preserve">              precision    recall  f1-score   support
+          -1       0.73      0.67      0.70        12
+           1       0.85      0.88      0.87        26
+    accuracy                           0.82        38
+   macro avg       0.79      0.78      0.78        38
+weighted avg       0.81      0.82      0.81        38
+</t>
+        </is>
+      </c>
+      <c r="R21" t="inlineStr">
+        <is>
+          <t>0.835135135135135 ∓ 0.031186742720077487</t>
+        </is>
+      </c>
+      <c r="S21" t="inlineStr">
+        <is>
+          <t>0.8329702881340548 ∓ 0.03246145226811514</t>
+        </is>
+      </c>
+      <c r="T21" t="inlineStr">
+        <is>
+          <t>0.8029930069930071 ∓ 0.04511343780163084</t>
+        </is>
+      </c>
+      <c r="U21" t="inlineStr">
+        <is>
+          <t>0.835307426360058 ∓ 0.034499414474537096</t>
+        </is>
+      </c>
+      <c r="V21" t="inlineStr">
+        <is>
+          <t>0.835135135135135 ∓ 0.031186742720077487</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>